<commit_message>
20.04.19 Today Sales Udated 9:08PM
</commit_message>
<xml_diff>
--- a/Othes/Cash.xlsx
+++ b/Othes/Cash.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Raju Ahamed" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -71,13 +71,10 @@
     <t>Distributor</t>
   </si>
   <si>
-    <t>Mithu Jaman</t>
+    <t>Date: 19.04.19</t>
   </si>
   <si>
-    <t>S.S Daffodils</t>
-  </si>
-  <si>
-    <t>Date: 17.04.19</t>
+    <t>Date: 20.04.19</t>
   </si>
 </sst>
 </file>
@@ -244,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -264,6 +261,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -324,6 +327,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1022,7 +1028,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -1033,7 +1039,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="47625" y="11191875"/>
+          <a:off x="47625" y="5353050"/>
           <a:ext cx="1190625" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1325,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1344,63 +1350,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="A4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -1410,10 +1416,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1428,13 +1434,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="11">
-        <v>68</v>
-      </c>
-      <c r="F6" s="11"/>
+      <c r="E6" s="13">
+        <v>43</v>
+      </c>
+      <c r="F6" s="13"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>68000</v>
+        <v>43000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -1447,13 +1453,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="11">
-        <v>135</v>
-      </c>
-      <c r="F7" s="11"/>
+      <c r="E7" s="13">
+        <v>88</v>
+      </c>
+      <c r="F7" s="13"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>67500</v>
+        <v>44000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1466,13 +1472,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="11">
-        <v>53</v>
-      </c>
-      <c r="F8" s="11"/>
+      <c r="E8" s="13">
+        <v>237</v>
+      </c>
+      <c r="F8" s="13"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>5300</v>
+        <v>23700</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1485,13 +1491,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="11">
-        <v>2</v>
-      </c>
-      <c r="F9" s="11"/>
+      <c r="E9" s="13">
+        <v>6</v>
+      </c>
+      <c r="F9" s="13"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1504,13 +1510,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="11">
-        <v>5</v>
-      </c>
-      <c r="F10" s="11"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -1523,8 +1527,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1537,14 +1541,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>141000</v>
+        <v>111000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -1587,60 +1591,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1650,11 +1654,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1729,60 +1733,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A30" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="A30" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:10" ht="27.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1791,10 +1795,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -1809,13 +1813,13 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="19">
-        <v>68</v>
-      </c>
-      <c r="F32" s="19"/>
+      <c r="E32" s="21">
+        <v>43</v>
+      </c>
+      <c r="F32" s="21"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
-        <v>68000</v>
+        <v>43000</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -1828,13 +1832,13 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="19">
-        <v>135</v>
-      </c>
-      <c r="F33" s="19"/>
+      <c r="E33" s="21">
+        <v>88</v>
+      </c>
+      <c r="F33" s="21"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
-        <v>67500</v>
+        <v>44000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -1847,13 +1851,13 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="19">
-        <v>53</v>
-      </c>
-      <c r="F34" s="19"/>
+      <c r="E34" s="21">
+        <v>237</v>
+      </c>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>5300</v>
+        <v>23700</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -1866,13 +1870,13 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="19">
-        <v>2</v>
-      </c>
-      <c r="F35" s="19"/>
+      <c r="E35" s="21">
+        <v>6</v>
+      </c>
+      <c r="F35" s="21"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -1885,13 +1889,11 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="19">
-        <v>5</v>
-      </c>
-      <c r="F36" s="19"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -1904,8 +1906,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1918,14 +1920,14 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="26"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
-        <v>141000</v>
+        <v>111000</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -1968,60 +1970,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="22"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="22" t="s">
+      <c r="H42" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="17"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="17" t="s">
+      <c r="H45" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2031,11 +2033,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2131,63 +2133,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2197,10 +2199,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2215,10 +2217,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="13">
         <v>68</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -2234,10 +2236,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="13">
         <v>135</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -2253,10 +2255,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="13">
         <v>53</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -2272,10 +2274,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="13">
         <v>2</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2291,10 +2293,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="13">
         <v>5</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2310,8 +2312,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2324,10 +2326,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -2374,76 +2376,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="27"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2518,60 +2520,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -2580,10 +2582,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -2598,10 +2600,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="21">
         <v>68</v>
       </c>
-      <c r="F32" s="19"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -2617,10 +2619,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E33" s="21">
         <v>135</v>
       </c>
-      <c r="F33" s="19"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -2636,10 +2638,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="21">
         <v>53</v>
       </c>
-      <c r="F34" s="19"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -2655,10 +2657,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="19">
+      <c r="E35" s="21">
         <v>2</v>
       </c>
-      <c r="F35" s="19"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2674,10 +2676,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="19">
+      <c r="E36" s="21">
         <v>5</v>
       </c>
-      <c r="F36" s="19"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2693,8 +2695,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2707,10 +2709,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="31"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -2757,76 +2759,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="22"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="22" t="s">
+      <c r="H42" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="17"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="17" t="s">
+      <c r="H45" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="28"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2906,8 +2908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection sqref="A1:J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2925,63 +2927,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2991,10 +2993,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3009,10 +3011,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="13">
         <v>44</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -3028,13 +3030,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="11">
-        <v>116</v>
-      </c>
-      <c r="F7" s="11"/>
+      <c r="E7" s="13">
+        <v>118</v>
+      </c>
+      <c r="F7" s="13"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>58000</v>
+        <v>59000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -3047,13 +3049,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="11">
-        <v>500</v>
-      </c>
-      <c r="F8" s="11"/>
+      <c r="E8" s="13">
+        <v>510</v>
+      </c>
+      <c r="F8" s="13"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>50000</v>
+        <v>51000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -3066,8 +3068,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3083,8 +3085,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3100,8 +3102,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3114,14 +3116,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>152000</v>
+        <v>154000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -3164,76 +3166,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="17"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="30"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3308,73 +3306,73 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-    </row>
-    <row r="31" spans="1:10" ht="20.25">
+      <c r="A30" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+    </row>
+    <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="9" t="s">
+      <c r="F31" s="17"/>
+      <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="6"/>
@@ -3385,14 +3383,14 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="2">
+      <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="13">
         <v>44</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="2">
+      <c r="F32" s="13"/>
+      <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
       </c>
@@ -3400,54 +3398,54 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:10" ht="20.25">
+    <row r="33" spans="1:10" ht="23.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="2">
+      <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="19">
-        <v>116</v>
-      </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="2">
+      <c r="E33" s="13">
+        <v>118</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="11">
         <f t="shared" si="1"/>
-        <v>58000</v>
+        <v>59000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" ht="20.25">
+    <row r="34" spans="1:10" ht="23.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="2">
+      <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="19">
-        <v>500</v>
-      </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="2">
+      <c r="E34" s="13">
+        <v>510</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="11">
         <f t="shared" si="1"/>
-        <v>50000</v>
+        <v>51000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="1:10" ht="20.25">
+    <row r="35" spans="1:10" ht="23.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="2">
+      <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="2">
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3455,16 +3453,16 @@
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" ht="20.25">
+    <row r="36" spans="1:10" ht="23.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="2">
+      <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="2">
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3472,16 +3470,16 @@
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:10" ht="20.25">
+    <row r="37" spans="1:10" ht="23.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="2">
+      <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="2">
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3489,18 +3487,18 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:10" ht="20.25">
+    <row r="38" spans="1:10" ht="23.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9">
+      <c r="E38" s="33"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
-        <v>152000</v>
+        <v>154000</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3543,76 +3541,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="22"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="22" t="s">
+      <c r="H42" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="17"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="17" t="s">
+      <c r="H45" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="28"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>

</xml_diff>

<commit_message>
21.04.19 Today last sales Updated
</commit_message>
<xml_diff>
--- a/Othes/Cash.xlsx
+++ b/Othes/Cash.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Raju Ahamed" sheetId="1" r:id="rId1"/>
     <sheet name="A.M Tipu" sheetId="2" r:id="rId2"/>
     <sheet name="Mithu Jaman" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="17">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -45,9 +46,6 @@
   </si>
   <si>
     <t>RECEIVED BY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raju Ahamed </t>
   </si>
   <si>
     <t>CASH READY BY</t>
@@ -74,7 +72,7 @@
     <t>Date: 19.04.19</t>
   </si>
   <si>
-    <t>Date: 20.04.19</t>
+    <t>Date: 21.04.19</t>
   </si>
 </sst>
 </file>
@@ -241,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -270,28 +268,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -303,16 +286,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -324,11 +334,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,6 +1051,187 @@
         <a:xfrm>
           <a:off x="47625" y="5353050"/>
           <a:ext cx="1190625" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Connector 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="5353050"/>
+          <a:ext cx="1190625" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6953250" y="5334000"/>
+          <a:ext cx="1466850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="12268200"/>
+          <a:ext cx="1228725" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6962775" y="12249150"/>
+          <a:ext cx="1457325" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1321,7 +1512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1331,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1350,63 +1541,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="A3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="A4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -1416,10 +1607,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1434,13 +1625,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="13">
-        <v>43</v>
-      </c>
-      <c r="F6" s="13"/>
+      <c r="E6" s="32">
+        <v>33</v>
+      </c>
+      <c r="F6" s="32"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>43000</v>
+        <v>33000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -1453,13 +1644,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="13">
-        <v>88</v>
-      </c>
-      <c r="F7" s="13"/>
+      <c r="E7" s="32">
+        <v>103</v>
+      </c>
+      <c r="F7" s="32"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>44000</v>
+        <v>51500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1472,13 +1663,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="13">
-        <v>237</v>
-      </c>
-      <c r="F8" s="13"/>
+      <c r="E8" s="32">
+        <v>129</v>
+      </c>
+      <c r="F8" s="32"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>23700</v>
+        <v>12900</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1491,13 +1682,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="13">
-        <v>6</v>
-      </c>
-      <c r="F9" s="13"/>
+      <c r="E9" s="32">
+        <v>12</v>
+      </c>
+      <c r="F9" s="32"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1510,8 +1701,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1527,8 +1718,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1541,14 +1732,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>111000</v>
+        <v>98000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -1591,60 +1782,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="H16" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
+      <c r="H19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1654,11 +1843,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
+      <c r="H20" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1733,60 +1922,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="A29" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A30" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="A30" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="27.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1795,10 +1984,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="27"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -1813,13 +2002,13 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
-        <v>43</v>
-      </c>
-      <c r="F32" s="21"/>
+      <c r="E32" s="28">
+        <v>33</v>
+      </c>
+      <c r="F32" s="28"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
-        <v>43000</v>
+        <v>33000</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -1832,13 +2021,13 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
-        <v>88</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="28">
+        <v>103</v>
+      </c>
+      <c r="F33" s="28"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
-        <v>44000</v>
+        <v>51500</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -1851,13 +2040,13 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
-        <v>237</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="28">
+        <v>129</v>
+      </c>
+      <c r="F34" s="28"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>23700</v>
+        <v>12900</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -1870,13 +2059,13 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
-        <v>6</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="28">
+        <v>12</v>
+      </c>
+      <c r="F35" s="28"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -1889,10 +2078,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="2">
-        <f t="shared" si="1"/>
+        <f>SUM(D36*E36)</f>
         <v>0</v>
       </c>
       <c r="H36" s="6"/>
@@ -1906,8 +2095,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1920,14 +2109,14 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="26"/>
+      <c r="D38" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="22"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
-        <v>111000</v>
+        <v>98000</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -1970,60 +2159,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
+      <c r="H42" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="19"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
+      <c r="H45" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2033,11 +2220,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
+      <c r="H46" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2065,6 +2252,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A42:B42"/>
@@ -2081,28 +2290,6 @@
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0.5" right="0" top="0.25" bottom="0" header="0.3" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -2133,63 +2320,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="A3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2199,10 +2386,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2217,10 +2404,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="32">
         <v>68</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -2236,10 +2423,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="32">
         <v>135</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -2255,10 +2442,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="32">
         <v>53</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -2274,10 +2461,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="32">
         <v>2</v>
       </c>
-      <c r="F9" s="13"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2293,10 +2480,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="32">
         <v>5</v>
       </c>
-      <c r="F10" s="13"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2312,8 +2499,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2326,10 +2513,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -2376,76 +2563,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="H16" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="19"/>
+      <c r="A19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="20"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
+      <c r="H19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="29"/>
+      <c r="A20" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="33"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
+      <c r="H20" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2520,60 +2707,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="A29" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -2582,10 +2769,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="27"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -2600,10 +2787,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="28">
         <v>68</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -2619,10 +2806,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="28">
         <v>135</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -2638,10 +2825,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="28">
         <v>53</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -2657,10 +2844,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="28">
         <v>2</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2676,10 +2863,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="28">
         <v>5</v>
       </c>
-      <c r="F36" s="21"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2695,8 +2882,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2709,10 +2896,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="31"/>
+      <c r="D38" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="35"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -2759,76 +2946,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
+      <c r="H42" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="19"/>
+      <c r="A45" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="20"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
+      <c r="H45" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46" s="30"/>
+      <c r="A46" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="34"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
+      <c r="H46" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2856,6 +3043,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -2872,30 +3083,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -2927,63 +3114,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="A3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="A4" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2993,10 +3180,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3011,10 +3198,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="32">
         <v>44</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -3030,10 +3217,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="32">
         <v>118</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -3049,10 +3236,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="32">
         <v>510</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -3068,8 +3255,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3085,8 +3272,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3102,8 +3289,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3116,10 +3303,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3166,72 +3353,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="H16" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
+      <c r="H19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
+      <c r="H20" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3306,60 +3493,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="A29" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="A30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -3368,10 +3555,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="29"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -3386,10 +3573,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="32">
         <v>44</v>
       </c>
-      <c r="F32" s="13"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -3405,10 +3592,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="32">
         <v>118</v>
       </c>
-      <c r="F33" s="13"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -3424,10 +3611,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="32">
         <v>510</v>
       </c>
-      <c r="F34" s="13"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -3443,8 +3630,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3460,8 +3647,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3477,8 +3664,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3491,10 +3678,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="33"/>
+      <c r="D38" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="36"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -3541,72 +3728,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
+      <c r="H42" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
+      <c r="H45" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
+      <c r="H46" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3634,16 +3821,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -3656,12 +3851,777 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+  </mergeCells>
+  <printOptions verticalCentered="1"/>
+  <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="31.5">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" ht="18">
+      <c r="A2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="1:10" ht="18">
+      <c r="A3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75">
+      <c r="A4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="1:10" ht="23.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="23.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="13">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="32">
+        <v>33</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="13">
+        <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
+        <v>33000</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="23.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="13">
+        <v>500</v>
+      </c>
+      <c r="E7" s="32">
+        <v>103</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="13">
+        <f t="shared" si="0"/>
+        <v>51500</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="23.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="13">
+        <v>100</v>
+      </c>
+      <c r="E8" s="32">
+        <v>129</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="13">
+        <f t="shared" si="0"/>
+        <v>12900</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="23.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="13">
+        <v>50</v>
+      </c>
+      <c r="E9" s="32">
+        <v>12</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="13">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="23.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="13">
+        <v>20</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="23.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="13">
+        <v>10</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="23.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14">
+        <f>SUM(G6:G11)</f>
+        <v>98000</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" ht="31.5">
+      <c r="A27" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+    </row>
+    <row r="28" spans="1:10" ht="18">
+      <c r="A28" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+    </row>
+    <row r="29" spans="1:10" ht="18.75">
+      <c r="A29" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+    </row>
+    <row r="30" spans="1:10" ht="18.75">
+      <c r="A30" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+    </row>
+    <row r="31" spans="1:10" ht="20.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="27"/>
+      <c r="G31" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" ht="20.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="15">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="28">
+        <v>33</v>
+      </c>
+      <c r="F32" s="28"/>
+      <c r="G32" s="15">
+        <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
+        <v>33000</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" ht="20.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="15">
+        <v>500</v>
+      </c>
+      <c r="E33" s="28">
+        <v>103</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="G33" s="15">
+        <f t="shared" si="1"/>
+        <v>51500</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" ht="20.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="15">
+        <v>100</v>
+      </c>
+      <c r="E34" s="28">
+        <v>129</v>
+      </c>
+      <c r="F34" s="28"/>
+      <c r="G34" s="15">
+        <f t="shared" si="1"/>
+        <v>12900</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="20.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="15">
+        <v>50</v>
+      </c>
+      <c r="E35" s="28">
+        <v>12</v>
+      </c>
+      <c r="F35" s="28"/>
+      <c r="G35" s="15">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="20.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="15">
+        <v>20</v>
+      </c>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="15">
+        <f>SUM(D36*E36)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" ht="20.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="15">
+        <v>10</v>
+      </c>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:10" ht="20.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="22"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16">
+        <f>SUM(G32:G37)</f>
+        <v>98000</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75">
+      <c r="A42" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="A17:B18"/>
     <mergeCell ref="H17:J18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -3669,15 +4629,8 @@
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
-  <printOptions verticalCentered="1"/>
-  <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
23.04.19 Today 10:27 PM Lasted sales Updated
</commit_message>
<xml_diff>
--- a/Othes/Cash.xlsx
+++ b/Othes/Cash.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="19">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Date: 22.04.19</t>
+  </si>
+  <si>
+    <t>Date: 23.04.19</t>
   </si>
 </sst>
 </file>
@@ -242,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -274,10 +277,37 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -289,43 +319,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -337,11 +340,17 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1515,7 +1524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1544,63 +1553,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -1610,10 +1619,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1628,10 +1637,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="17">
         <v>33</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>33000</v>
@@ -1647,10 +1656,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="17">
         <v>103</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>51500</v>
@@ -1666,10 +1675,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="17">
         <v>129</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>12900</v>
@@ -1685,10 +1694,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="17">
         <v>12</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>600</v>
@@ -1704,8 +1713,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1721,8 +1730,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1735,10 +1744,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -1785,58 +1794,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1846,11 +1855,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1925,60 +1934,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="27.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1987,10 +1996,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="27"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -2005,10 +2014,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="25">
         <v>33</v>
       </c>
-      <c r="F32" s="28"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>33000</v>
@@ -2024,10 +2033,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="25">
         <v>103</v>
       </c>
-      <c r="F33" s="28"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>51500</v>
@@ -2043,10 +2052,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="28">
+      <c r="E34" s="25">
         <v>129</v>
       </c>
-      <c r="F34" s="28"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>12900</v>
@@ -2062,10 +2071,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="28">
+      <c r="E35" s="25">
         <v>12</v>
       </c>
-      <c r="F35" s="28"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>600</v>
@@ -2081,8 +2090,8 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="2">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2098,8 +2107,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2112,10 +2121,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="22"/>
+      <c r="E38" s="30"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -2162,58 +2171,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="19" t="s">
+      <c r="H42" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2223,11 +2232,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2255,28 +2264,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A42:B42"/>
@@ -2293,6 +2280,28 @@
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0.5" right="0" top="0.25" bottom="0" header="0.3" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -2323,63 +2332,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2389,10 +2398,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2407,10 +2416,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="17">
         <v>68</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -2426,10 +2435,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="17">
         <v>135</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -2445,10 +2454,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="17">
         <v>53</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -2464,10 +2473,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="17">
         <v>2</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2483,10 +2492,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="17">
         <v>5</v>
       </c>
-      <c r="F10" s="32"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2502,8 +2511,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2516,10 +2525,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -2566,60 +2575,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="20"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="33" t="s">
@@ -2631,11 +2640,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2710,60 +2719,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -2772,10 +2781,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="27"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -2790,10 +2799,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="25">
         <v>68</v>
       </c>
-      <c r="F32" s="28"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -2809,10 +2818,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="25">
         <v>135</v>
       </c>
-      <c r="F33" s="28"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -2828,10 +2837,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="28">
+      <c r="E34" s="25">
         <v>53</v>
       </c>
-      <c r="F34" s="28"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -2847,10 +2856,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="28">
+      <c r="E35" s="25">
         <v>2</v>
       </c>
-      <c r="F35" s="28"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2866,10 +2875,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="28">
+      <c r="E36" s="25">
         <v>5</v>
       </c>
-      <c r="F36" s="28"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2885,8 +2894,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2949,60 +2958,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="19" t="s">
+      <c r="H42" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="20"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="34" t="s">
@@ -3014,11 +3023,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3046,30 +3055,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3086,6 +3071,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3117,63 +3126,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3183,10 +3192,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3201,10 +3210,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="17">
         <v>44</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -3220,10 +3229,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="17">
         <v>118</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -3239,10 +3248,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="17">
         <v>510</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -3258,8 +3267,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3275,8 +3284,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3292,8 +3301,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3306,10 +3315,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3356,72 +3365,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3496,60 +3505,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -3558,10 +3567,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="29" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="29"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -3576,10 +3585,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="17">
         <v>44</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="17"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -3595,10 +3604,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="17">
         <v>118</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="17"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -3614,10 +3623,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="17">
         <v>510</v>
       </c>
-      <c r="F34" s="32"/>
+      <c r="F34" s="17"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -3633,8 +3642,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3650,8 +3659,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3667,8 +3676,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3681,10 +3690,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="36"/>
+      <c r="E38" s="37"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -3731,58 +3740,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="19" t="s">
+      <c r="H42" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="34"/>
@@ -3792,11 +3801,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3824,24 +3833,16 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -3854,766 +3855,6 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-  </mergeCells>
-  <printOptions verticalCentered="1"/>
-  <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J48"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection sqref="A1:J47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-    </row>
-    <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-    </row>
-    <row r="5" spans="1:10" ht="23.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" ht="23.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="13">
-        <v>1000</v>
-      </c>
-      <c r="E6" s="32">
-        <v>20</v>
-      </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="13">
-        <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>20000</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" ht="23.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="13">
-        <v>500</v>
-      </c>
-      <c r="E7" s="32">
-        <v>66</v>
-      </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="13">
-        <f t="shared" si="0"/>
-        <v>33000</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="23.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="13">
-        <v>100</v>
-      </c>
-      <c r="E8" s="32">
-        <v>181</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="13">
-        <f t="shared" si="0"/>
-        <v>18100</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="23.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="13">
-        <v>50</v>
-      </c>
-      <c r="E9" s="32">
-        <v>38</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="13">
-        <f t="shared" si="0"/>
-        <v>1900</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" ht="23.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="13">
-        <v>20</v>
-      </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" ht="23.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="13">
-        <v>10</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" ht="23.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14">
-        <f>SUM(G6:G11)</f>
-        <v>73000</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-    </row>
-    <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-    </row>
-    <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-    </row>
-    <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-    </row>
-    <row r="31" spans="1:10" ht="20.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="27"/>
-      <c r="G31" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" ht="20.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="15">
-        <v>1000</v>
-      </c>
-      <c r="E32" s="28">
-        <v>20</v>
-      </c>
-      <c r="F32" s="28"/>
-      <c r="G32" s="15">
-        <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
-        <v>20000</v>
-      </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" ht="20.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="15">
-        <v>500</v>
-      </c>
-      <c r="E33" s="28">
-        <v>66</v>
-      </c>
-      <c r="F33" s="28"/>
-      <c r="G33" s="15">
-        <f t="shared" si="1"/>
-        <v>33000</v>
-      </c>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="1:10" ht="20.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="15">
-        <v>100</v>
-      </c>
-      <c r="E34" s="28">
-        <v>181</v>
-      </c>
-      <c r="F34" s="28"/>
-      <c r="G34" s="15">
-        <f t="shared" si="1"/>
-        <v>18100</v>
-      </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="1:10" ht="20.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="15">
-        <v>50</v>
-      </c>
-      <c r="E35" s="28">
-        <v>38</v>
-      </c>
-      <c r="F35" s="28"/>
-      <c r="G35" s="15">
-        <f t="shared" si="1"/>
-        <v>1900</v>
-      </c>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:10" ht="20.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="15">
-        <v>20</v>
-      </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="15">
-        <f>SUM(D36*E36)</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="1:10" ht="20.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="15">
-        <v>10</v>
-      </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="1:10" ht="20.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="22"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16">
-        <f>SUM(G32:G37)</f>
-        <v>73000</v>
-      </c>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-    </row>
-    <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="A17:B18"/>
@@ -4633,6 +3874,775 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
   </mergeCells>
+  <printOptions verticalCentered="1"/>
+  <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection sqref="A1:J47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="31.5">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" ht="18">
+      <c r="A2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" ht="18">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75">
+      <c r="A4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="1:10" ht="23.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="23.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="13">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="17">
+        <v>50</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="13">
+        <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
+        <v>50000</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="23.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="13">
+        <v>500</v>
+      </c>
+      <c r="E7" s="17">
+        <v>116</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="13">
+        <f t="shared" si="0"/>
+        <v>58000</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="23.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="13">
+        <v>100</v>
+      </c>
+      <c r="E8" s="17">
+        <v>151</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="13">
+        <f t="shared" si="0"/>
+        <v>15100</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="23.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="13">
+        <v>50</v>
+      </c>
+      <c r="E9" s="17">
+        <v>58</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="13">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="23.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="13">
+        <v>20</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="23.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="13">
+        <v>10</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="23.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14">
+        <f>SUM(G6:G11)</f>
+        <v>126000</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" ht="31.5">
+      <c r="A27" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="1:10" ht="18">
+      <c r="A28" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+    </row>
+    <row r="29" spans="1:10" ht="18.75">
+      <c r="A29" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+    </row>
+    <row r="30" spans="1:10" ht="18.75">
+      <c r="A30" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="16">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="17">
+        <v>50</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="16">
+        <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
+        <v>50000</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="16">
+        <v>500</v>
+      </c>
+      <c r="E33" s="17">
+        <v>116</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="16">
+        <f t="shared" si="1"/>
+        <v>58000</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="16">
+        <v>100</v>
+      </c>
+      <c r="E34" s="17">
+        <v>151</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="16">
+        <f t="shared" si="1"/>
+        <v>15100</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="16">
+        <v>50</v>
+      </c>
+      <c r="E35" s="17">
+        <v>58</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="16">
+        <f t="shared" si="1"/>
+        <v>2900</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="16">
+        <v>20</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="16">
+        <f>SUM(D36*E36)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="16">
+        <v>10</v>
+      </c>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="39"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15">
+        <f>SUM(G32:G37)</f>
+        <v>126000</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75">
+      <c r="A42" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75">
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+  </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
30.04.19 today Last 12:28am Updated
</commit_message>
<xml_diff>
--- a/Othes/Cash.xlsx
+++ b/Othes/Cash.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Raju Ahamed" sheetId="1" r:id="rId1"/>
-    <sheet name="A.M Tipu" sheetId="2" r:id="rId2"/>
-    <sheet name="Mithu Jaman" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Raju Ahamed" sheetId="1" r:id="rId2"/>
+    <sheet name="A.M Tipu" sheetId="2" r:id="rId3"/>
+    <sheet name="Mithu Jaman" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -78,7 +78,7 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 29.04.19</t>
+    <t>Date: 30.04.19</t>
   </si>
 </sst>
 </file>
@@ -283,16 +283,46 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -301,34 +331,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -345,12 +351,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -370,6 +370,187 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Connector 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="5353050"/>
+          <a:ext cx="1190625" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6953250" y="5334000"/>
+          <a:ext cx="1466850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="12268200"/>
+          <a:ext cx="1228725" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6962775" y="12249150"/>
+          <a:ext cx="1457325" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -550,7 +731,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -775,7 +956,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1063,187 +1244,6 @@
         <a:xfrm>
           <a:off x="47625" y="5353050"/>
           <a:ext cx="1190625" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Straight Connector 1"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="47625" y="5353050"/>
-          <a:ext cx="1190625" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6953250" y="5334000"/>
-          <a:ext cx="1466850" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>11113</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Connector 3"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9525" y="12268200"/>
-          <a:ext cx="1228725" cy="1588"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Connector 4"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6962775" y="12249150"/>
-          <a:ext cx="1457325" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1532,10 +1532,778 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="31.5">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" ht="18">
+      <c r="A2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" ht="18">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75">
+      <c r="A4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" spans="1:10" ht="23.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="23.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="13">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="21">
+        <v>50</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="13">
+        <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
+        <v>50000</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="23.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="13">
+        <v>500</v>
+      </c>
+      <c r="E7" s="21">
+        <v>16</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="13">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="23.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="13">
+        <v>100</v>
+      </c>
+      <c r="E8" s="21">
+        <v>151</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="13">
+        <f t="shared" si="0"/>
+        <v>15100</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="23.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="13">
+        <v>50</v>
+      </c>
+      <c r="E9" s="21">
+        <v>58</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="13">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="23.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="13">
+        <v>20</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="23.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="13">
+        <v>10</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="23.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14">
+        <f>SUM(G6:G11)</f>
+        <v>76000</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" ht="31.5">
+      <c r="A27" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="1:10" ht="18">
+      <c r="A28" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+    </row>
+    <row r="29" spans="1:10" ht="18.75">
+      <c r="A29" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+    </row>
+    <row r="30" spans="1:10" ht="18.75">
+      <c r="A30" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="16">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="21">
+        <v>50</v>
+      </c>
+      <c r="F32" s="21"/>
+      <c r="G32" s="16">
+        <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
+        <v>50000</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="16">
+        <v>500</v>
+      </c>
+      <c r="E33" s="21">
+        <v>116</v>
+      </c>
+      <c r="F33" s="21"/>
+      <c r="G33" s="16">
+        <f t="shared" si="1"/>
+        <v>58000</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="16">
+        <v>100</v>
+      </c>
+      <c r="E34" s="21">
+        <v>151</v>
+      </c>
+      <c r="F34" s="21"/>
+      <c r="G34" s="16">
+        <f t="shared" si="1"/>
+        <v>15100</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="16">
+        <v>50</v>
+      </c>
+      <c r="E35" s="21">
+        <v>58</v>
+      </c>
+      <c r="F35" s="21"/>
+      <c r="G35" s="16">
+        <f t="shared" si="1"/>
+        <v>2900</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="16">
+        <v>20</v>
+      </c>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="16">
+        <f>SUM(D36*E36)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="16">
+        <v>10</v>
+      </c>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="29"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15">
+        <f>SUM(G32:G37)</f>
+        <v>126000</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75">
+      <c r="A42" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="30"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75">
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+  </mergeCells>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
+  <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection sqref="A1:J47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1553,63 +2321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -1619,10 +2387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1637,13 +2405,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="32">
-        <v>62</v>
-      </c>
-      <c r="F6" s="32"/>
+      <c r="E6" s="21">
+        <v>89</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>62000</v>
+        <v>89000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -1656,13 +2424,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="32">
-        <v>90</v>
-      </c>
-      <c r="F7" s="32"/>
+      <c r="E7" s="21">
+        <v>75</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>45000</v>
+        <v>37500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1675,13 +2443,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="32">
-        <v>150</v>
-      </c>
-      <c r="F8" s="32"/>
+      <c r="E8" s="21">
+        <v>325</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>15000</v>
+        <v>32500</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1694,8 +2462,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1711,8 +2479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1728,8 +2496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1742,14 +2510,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>122000</v>
+        <v>159000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -1792,58 +2560,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1853,11 +2621,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1944,60 +2712,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6"/>
@@ -2006,10 +2774,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2024,13 +2792,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="28">
-        <v>62</v>
-      </c>
-      <c r="F33" s="28"/>
+      <c r="E33" s="34">
+        <v>89</v>
+      </c>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>62000</v>
+        <v>89000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2043,13 +2811,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="28">
-        <v>90</v>
-      </c>
-      <c r="F34" s="28"/>
+      <c r="E34" s="34">
+        <v>75</v>
+      </c>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>45000</v>
+        <v>37500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2062,13 +2830,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="28">
-        <v>150</v>
-      </c>
-      <c r="F35" s="28"/>
+      <c r="E35" s="34">
+        <v>325</v>
+      </c>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>32500</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2081,8 +2849,8 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2098,8 +2866,8 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -2115,8 +2883,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2129,14 +2897,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="22"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>122000</v>
+        <v>159000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2179,58 +2947,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="19"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="19" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2240,11 +3008,11 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17" t="s">
+      <c r="H47" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -2317,7 +3085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K48"/>
   <sheetViews>
@@ -2340,63 +3108,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2406,10 +3174,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2424,10 +3192,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -2443,10 +3211,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -2462,10 +3230,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -2481,10 +3249,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2500,10 +3268,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="32"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -2519,8 +3287,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2533,10 +3301,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -2583,76 +3351,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="20"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2727,60 +3495,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -2789,10 +3557,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="27"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -2807,10 +3575,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="28"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -2826,10 +3594,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="28"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -2845,10 +3613,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="28">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="28"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -2864,10 +3632,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="28">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="28"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2883,10 +3651,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="28">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="28"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2902,8 +3670,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2916,10 +3684,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="37"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -2966,76 +3734,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="19" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="20"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="34"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3111,7 +3879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K48"/>
   <sheetViews>
@@ -3134,63 +3902,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3200,10 +3968,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3218,10 +3986,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -3237,10 +4005,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -3256,10 +4024,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -3275,8 +4043,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3292,8 +4060,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3309,8 +4077,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3323,10 +4091,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3373,72 +4141,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3513,60 +4281,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -3575,10 +4343,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="29" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="29"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -3593,10 +4361,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -3612,10 +4380,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -3631,10 +4399,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="32"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -3650,8 +4418,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3667,8 +4435,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3684,8 +4452,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3698,10 +4466,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="36"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -3748,72 +4516,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="19" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3887,772 +4655,4 @@
   <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J48"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-    </row>
-    <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-    </row>
-    <row r="5" spans="1:10" ht="23.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" ht="23.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="13">
-        <v>1000</v>
-      </c>
-      <c r="E6" s="32">
-        <v>50</v>
-      </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="13">
-        <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>50000</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" ht="23.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="13">
-        <v>500</v>
-      </c>
-      <c r="E7" s="32">
-        <v>116</v>
-      </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="13">
-        <f t="shared" si="0"/>
-        <v>58000</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="23.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="13">
-        <v>100</v>
-      </c>
-      <c r="E8" s="32">
-        <v>151</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="13">
-        <f t="shared" si="0"/>
-        <v>15100</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="23.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="13">
-        <v>50</v>
-      </c>
-      <c r="E9" s="32">
-        <v>58</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="13">
-        <f t="shared" si="0"/>
-        <v>2900</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" ht="23.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="13">
-        <v>20</v>
-      </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" ht="23.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="13">
-        <v>10</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" ht="23.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14">
-        <f>SUM(G6:G11)</f>
-        <v>126000</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-    </row>
-    <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-    </row>
-    <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-    </row>
-    <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-    </row>
-    <row r="31" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="16">
-        <v>1000</v>
-      </c>
-      <c r="E32" s="32">
-        <v>50</v>
-      </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="16">
-        <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
-        <v>50000</v>
-      </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="16">
-        <v>500</v>
-      </c>
-      <c r="E33" s="32">
-        <v>116</v>
-      </c>
-      <c r="F33" s="32"/>
-      <c r="G33" s="16">
-        <f t="shared" si="1"/>
-        <v>58000</v>
-      </c>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="16">
-        <v>100</v>
-      </c>
-      <c r="E34" s="32">
-        <v>151</v>
-      </c>
-      <c r="F34" s="32"/>
-      <c r="G34" s="16">
-        <f t="shared" si="1"/>
-        <v>15100</v>
-      </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="16">
-        <v>50</v>
-      </c>
-      <c r="E35" s="32">
-        <v>58</v>
-      </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="16">
-        <f t="shared" si="1"/>
-        <v>2900</v>
-      </c>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="16">
-        <v>20</v>
-      </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="16">
-        <f>SUM(D36*E36)</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="16">
-        <v>10</v>
-      </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15">
-        <f>SUM(G32:G37)</f>
-        <v>126000</v>
-      </c>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-    </row>
-    <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-  </mergeCells>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
-  <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>